<commit_message>
Total Masters Working Fine
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/WMPS_EXCELData.xlsx
+++ b/src/test/resources/ExcelData/WMPS_EXCELData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15090" windowHeight="3225" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15090" windowHeight="3225" firstSheet="13" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Date" sheetId="31" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="448">
   <si>
     <t>Material_Type</t>
   </si>
@@ -1274,12 +1274,6 @@
     <t xml:space="preserve">IN - INDIA </t>
   </si>
   <si>
-    <t xml:space="preserve">MYSORE </t>
-  </si>
-  <si>
-    <t>HeteroManPower1</t>
-  </si>
-  <si>
     <t>30022023</t>
   </si>
   <si>
@@ -1307,15 +1301,6 @@
     <t>Date6ML</t>
   </si>
   <si>
-    <t>06112023</t>
-  </si>
-  <si>
-    <t>30062023</t>
-  </si>
-  <si>
-    <t>25052023</t>
-  </si>
-  <si>
     <t>BronzeNitroChloride</t>
   </si>
   <si>
@@ -1349,18 +1334,6 @@
     <t>DCInvoiceNumber_Edit</t>
   </si>
   <si>
-    <t>29042023</t>
-  </si>
-  <si>
-    <t>45RW_MonuChloride</t>
-  </si>
-  <si>
-    <t>45RW_MC_Manufacturer</t>
-  </si>
-  <si>
-    <t>45RW_MC_Supplier</t>
-  </si>
-  <si>
     <t>PO-679635065A111</t>
   </si>
   <si>
@@ -1395,6 +1368,36 @@
   </si>
   <si>
     <t>FP-600</t>
+  </si>
+  <si>
+    <t>Intermediate</t>
+  </si>
+  <si>
+    <t>18122023</t>
+  </si>
+  <si>
+    <t>25032024</t>
+  </si>
+  <si>
+    <t>25062024</t>
+  </si>
+  <si>
+    <t>25042024</t>
+  </si>
+  <si>
+    <t>69_AcetalDehyde</t>
+  </si>
+  <si>
+    <t>69_AcetalDehyde_Manufacturer</t>
+  </si>
+  <si>
+    <t>69_AcetalDehyde_Supplier</t>
+  </si>
+  <si>
+    <t>HeteroAcetalDehyde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kolar </t>
   </si>
 </sst>
 </file>
@@ -1820,17 +1823,18 @@
   <dimension ref="A1:AX11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>382</v>
       </c>
@@ -1844,584 +1848,35 @@
         <v>384</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2"/>
-      <c r="AF1" s="2"/>
-      <c r="AG1" s="2"/>
-      <c r="AH1" s="2"/>
-      <c r="AI1" s="2"/>
-      <c r="AJ1" s="2"/>
-      <c r="AK1" s="2"/>
-      <c r="AL1" s="2"/>
-      <c r="AM1" s="2"/>
-      <c r="AN1" s="2"/>
-      <c r="AO1" s="2"/>
-      <c r="AP1" s="2"/>
-      <c r="AQ1" s="2"/>
-      <c r="AR1" s="2"/>
-      <c r="AS1" s="2"/>
-      <c r="AT1" s="2"/>
-      <c r="AU1" s="2"/>
-      <c r="AV1" s="2"/>
-      <c r="AW1" s="2"/>
-      <c r="AX1" s="2"/>
-    </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="2" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>431</v>
+        <v>439</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>419</v>
+        <v>440</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>418</v>
+        <v>442</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
-      <c r="AF2" s="2"/>
-      <c r="AG2" s="2"/>
-      <c r="AH2" s="2"/>
-      <c r="AI2" s="2"/>
-      <c r="AJ2" s="2"/>
-      <c r="AK2" s="2"/>
-      <c r="AL2" s="2"/>
-      <c r="AM2" s="2"/>
-      <c r="AN2" s="2"/>
-      <c r="AO2" s="2"/>
-      <c r="AP2" s="2"/>
-      <c r="AQ2" s="2"/>
-      <c r="AR2" s="2"/>
-      <c r="AS2" s="2"/>
-      <c r="AT2" s="2"/>
-      <c r="AU2" s="2"/>
-      <c r="AV2" s="2"/>
-      <c r="AW2" s="2"/>
-      <c r="AX2" s="2"/>
-    </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
-      <c r="AE3" s="2"/>
-      <c r="AF3" s="2"/>
-      <c r="AG3" s="2"/>
-      <c r="AH3" s="2"/>
-      <c r="AI3" s="2"/>
-      <c r="AJ3" s="2"/>
-      <c r="AK3" s="2"/>
-      <c r="AL3" s="2"/>
-      <c r="AM3" s="2"/>
-      <c r="AN3" s="2"/>
-      <c r="AO3" s="2"/>
-      <c r="AP3" s="2"/>
-      <c r="AQ3" s="2"/>
-      <c r="AR3" s="2"/>
-      <c r="AS3" s="2"/>
-      <c r="AT3" s="2"/>
-      <c r="AU3" s="2"/>
-      <c r="AV3" s="2"/>
-      <c r="AW3" s="2"/>
-      <c r="AX3" s="2"/>
-    </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="2"/>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="2"/>
-      <c r="AE4" s="2"/>
-      <c r="AF4" s="2"/>
-      <c r="AG4" s="2"/>
-      <c r="AH4" s="2"/>
-      <c r="AI4" s="2"/>
-      <c r="AJ4" s="2"/>
-      <c r="AK4" s="2"/>
-      <c r="AL4" s="2"/>
-      <c r="AM4" s="2"/>
-      <c r="AN4" s="2"/>
-      <c r="AO4" s="2"/>
-      <c r="AP4" s="2"/>
-      <c r="AQ4" s="2"/>
-      <c r="AR4" s="2"/>
-      <c r="AS4" s="2"/>
-      <c r="AT4" s="2"/>
-      <c r="AU4" s="2"/>
-      <c r="AV4" s="2"/>
-      <c r="AW4" s="2"/>
-      <c r="AX4" s="2"/>
-    </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
-      <c r="AA5" s="2"/>
-      <c r="AB5" s="2"/>
-      <c r="AC5" s="2"/>
-      <c r="AD5" s="2"/>
-      <c r="AE5" s="2"/>
-      <c r="AF5" s="2"/>
-      <c r="AG5" s="2"/>
-      <c r="AH5" s="2"/>
-      <c r="AI5" s="2"/>
-      <c r="AJ5" s="2"/>
-      <c r="AK5" s="2"/>
-      <c r="AL5" s="2"/>
-      <c r="AM5" s="2"/>
-      <c r="AN5" s="2"/>
-      <c r="AO5" s="2"/>
-      <c r="AP5" s="2"/>
-      <c r="AQ5" s="2"/>
-      <c r="AR5" s="2"/>
-      <c r="AS5" s="2"/>
-      <c r="AT5" s="2"/>
-      <c r="AU5" s="2"/>
-      <c r="AV5" s="2"/>
-      <c r="AW5" s="2"/>
-      <c r="AX5" s="2"/>
-    </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
-      <c r="Z6" s="2"/>
-      <c r="AA6" s="2"/>
-      <c r="AB6" s="2"/>
-      <c r="AC6" s="2"/>
-      <c r="AD6" s="2"/>
-      <c r="AE6" s="2"/>
-      <c r="AF6" s="2"/>
-      <c r="AG6" s="2"/>
-      <c r="AH6" s="2"/>
-      <c r="AI6" s="2"/>
-      <c r="AJ6" s="2"/>
-      <c r="AK6" s="2"/>
-      <c r="AL6" s="2"/>
-      <c r="AM6" s="2"/>
-      <c r="AN6" s="2"/>
-      <c r="AO6" s="2"/>
-      <c r="AP6" s="2"/>
-      <c r="AQ6" s="2"/>
-      <c r="AR6" s="2"/>
-      <c r="AS6" s="2"/>
-      <c r="AT6" s="2"/>
-      <c r="AU6" s="2"/>
-      <c r="AV6" s="2"/>
-      <c r="AW6" s="2"/>
-      <c r="AX6" s="2"/>
-    </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
-      <c r="AA7" s="2"/>
-      <c r="AB7" s="2"/>
-      <c r="AC7" s="2"/>
-      <c r="AD7" s="2"/>
-      <c r="AE7" s="2"/>
-      <c r="AF7" s="2"/>
-      <c r="AG7" s="2"/>
-      <c r="AH7" s="2"/>
-      <c r="AI7" s="2"/>
-      <c r="AJ7" s="2"/>
-      <c r="AK7" s="2"/>
-      <c r="AL7" s="2"/>
-      <c r="AM7" s="2"/>
-      <c r="AN7" s="2"/>
-      <c r="AO7" s="2"/>
-      <c r="AP7" s="2"/>
-      <c r="AQ7" s="2"/>
-      <c r="AR7" s="2"/>
-      <c r="AS7" s="2"/>
-      <c r="AT7" s="2"/>
-      <c r="AU7" s="2"/>
-      <c r="AV7" s="2"/>
-      <c r="AW7" s="2"/>
-      <c r="AX7" s="2"/>
-    </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
-      <c r="AA8" s="2"/>
-      <c r="AB8" s="2"/>
-      <c r="AC8" s="2"/>
-      <c r="AD8" s="2"/>
-      <c r="AE8" s="2"/>
-      <c r="AF8" s="2"/>
-      <c r="AG8" s="2"/>
-      <c r="AH8" s="2"/>
-      <c r="AI8" s="2"/>
-      <c r="AJ8" s="2"/>
-      <c r="AK8" s="2"/>
-      <c r="AL8" s="2"/>
-      <c r="AM8" s="2"/>
-      <c r="AN8" s="2"/>
-      <c r="AO8" s="2"/>
-      <c r="AP8" s="2"/>
-      <c r="AQ8" s="2"/>
-      <c r="AR8" s="2"/>
-      <c r="AS8" s="2"/>
-      <c r="AT8" s="2"/>
-      <c r="AU8" s="2"/>
-      <c r="AV8" s="2"/>
-      <c r="AW8" s="2"/>
-      <c r="AX8" s="2"/>
-    </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="2"/>
-      <c r="Z9" s="2"/>
-      <c r="AA9" s="2"/>
-      <c r="AB9" s="2"/>
-      <c r="AC9" s="2"/>
-      <c r="AD9" s="2"/>
-      <c r="AE9" s="2"/>
-      <c r="AF9" s="2"/>
-      <c r="AG9" s="2"/>
-      <c r="AH9" s="2"/>
-      <c r="AI9" s="2"/>
-      <c r="AJ9" s="2"/>
-      <c r="AK9" s="2"/>
-      <c r="AL9" s="2"/>
-      <c r="AM9" s="2"/>
-      <c r="AN9" s="2"/>
-      <c r="AO9" s="2"/>
-      <c r="AP9" s="2"/>
-      <c r="AQ9" s="2"/>
-      <c r="AR9" s="2"/>
-      <c r="AS9" s="2"/>
-      <c r="AT9" s="2"/>
-      <c r="AU9" s="2"/>
-      <c r="AV9" s="2"/>
-      <c r="AW9" s="2"/>
-      <c r="AX9" s="2"/>
-    </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2"/>
-      <c r="Y10" s="2"/>
-      <c r="Z10" s="2"/>
-      <c r="AA10" s="2"/>
-      <c r="AB10" s="2"/>
-      <c r="AC10" s="2"/>
-      <c r="AD10" s="2"/>
-      <c r="AE10" s="2"/>
-      <c r="AF10" s="2"/>
-      <c r="AG10" s="2"/>
-      <c r="AH10" s="2"/>
-      <c r="AI10" s="2"/>
-      <c r="AJ10" s="2"/>
-      <c r="AK10" s="2"/>
-      <c r="AL10" s="2"/>
-      <c r="AM10" s="2"/>
-      <c r="AN10" s="2"/>
-      <c r="AO10" s="2"/>
-      <c r="AP10" s="2"/>
-      <c r="AQ10" s="2"/>
-      <c r="AR10" s="2"/>
-      <c r="AS10" s="2"/>
-      <c r="AT10" s="2"/>
-      <c r="AU10" s="2"/>
-      <c r="AV10" s="2"/>
-      <c r="AW10" s="2"/>
-      <c r="AX10" s="2"/>
-    </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-      <c r="X11" s="2"/>
-      <c r="Y11" s="2"/>
-      <c r="Z11" s="2"/>
-      <c r="AA11" s="2"/>
-      <c r="AB11" s="2"/>
-      <c r="AC11" s="2"/>
-      <c r="AD11" s="2"/>
-      <c r="AE11" s="2"/>
-      <c r="AF11" s="2"/>
-      <c r="AG11" s="2"/>
-      <c r="AH11" s="2"/>
-      <c r="AI11" s="2"/>
-      <c r="AJ11" s="2"/>
-      <c r="AK11" s="2"/>
-      <c r="AL11" s="2"/>
-      <c r="AM11" s="2"/>
-      <c r="AN11" s="2"/>
-      <c r="AO11" s="2"/>
-      <c r="AP11" s="2"/>
-      <c r="AQ11" s="2"/>
-      <c r="AR11" s="2"/>
-      <c r="AS11" s="2"/>
-      <c r="AT11" s="2"/>
-      <c r="AU11" s="2"/>
-      <c r="AV11" s="2"/>
-      <c r="AW11" s="2"/>
-      <c r="AX11" s="2"/>
-    </row>
+        <v>441</v>
+      </c>
+    </row>
+    <row r="3" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3359,25 +2814,26 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>401</v>
       </c>
@@ -3406,12 +2862,12 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>407</v>
+        <v>446</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>406</v>
+        <v>447</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>402</v>
@@ -3435,6 +2891,7 @@
         <v>268</v>
       </c>
     </row>
+    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3541,7 +2998,7 @@
         <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>260</v>
@@ -3805,10 +3262,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE5"/>
+  <dimension ref="A1:AE8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection sqref="A1:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3834,7 +3291,7 @@
     <col min="19" max="19" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>354</v>
       </c>
@@ -3892,20 +3349,8 @@
       <c r="S1" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2"/>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>299</v>
       </c>
@@ -3955,7 +3400,7 @@
         <v>88</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>324</v>
+        <v>438</v>
       </c>
       <c r="R2" s="4" t="s">
         <v>324</v>
@@ -3963,20 +3408,8 @@
       <c r="S2" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>299</v>
       </c>
@@ -4014,26 +3447,8 @@
         <v>335</v>
       </c>
       <c r="M3" s="5"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
-      <c r="AE3" s="2"/>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>299</v>
       </c>
@@ -4071,26 +3486,8 @@
         <v>335</v>
       </c>
       <c r="M4" s="5"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="2"/>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="2"/>
-      <c r="AE4" s="2"/>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>299</v>
       </c>
@@ -4128,25 +3525,10 @@
         <v>335</v>
       </c>
       <c r="M5" s="5"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
-      <c r="AA5" s="2"/>
-      <c r="AB5" s="2"/>
-      <c r="AC5" s="2"/>
-      <c r="AD5" s="2"/>
-      <c r="AE5" s="2"/>
-    </row>
+    </row>
+    <row r="6" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -4871,29 +4253,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.7109375" customWidth="1"/>
-    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4936,27 +4319,22 @@
       <c r="N1" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>255</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>432</v>
+        <v>443</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>433</v>
+        <v>444</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>434</v>
+        <v>445</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>332</v>
@@ -4968,30 +4346,25 @@
         <v>303</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>370</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>446</v>
-      </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>352</v>
@@ -4999,79 +4372,26 @@
       <c r="C3" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
       <c r="K3" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+    </row>
+    <row r="4" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F4" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
       <c r="K4" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="H9" s="2"/>
-    </row>
+    </row>
+    <row r="5" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5082,7 +4402,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5103,7 +4423,7 @@
         <v>301</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>264</v>
@@ -5141,7 +4461,7 @@
         <v>302</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>362</v>
@@ -5153,7 +4473,7 @@
         <v>400</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>291</v>
@@ -5168,7 +4488,7 @@
         <v>22</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -5386,7 +4706,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>253</v>
@@ -5442,22 +4762,22 @@
         <v>377</v>
       </c>
       <c r="D1" s="16" t="s">
+        <v>409</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>411</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>412</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>413</v>
       </c>
       <c r="G1" s="17" t="s">
         <v>396</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -5465,31 +4785,31 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>395</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -5557,7 +4877,7 @@
         <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>236</v>
@@ -5566,7 +4886,7 @@
         <v>63</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>386</v>
@@ -5583,23 +4903,23 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="4" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>235</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>235</v>

</xml_diff>